<commit_message>
Cabeceras corregidas para algoritmos de firma y verificación
</commit_message>
<xml_diff>
--- a/Proyecto1/times_RCA_PDD_DSA_ECDSA.xlsx
+++ b/Proyecto1/times_RCA_PDD_DSA_ECDSA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AbrilVzqz/Documents/Facultad de Ingeniería/10Semestre/Criptografía/Proyecto1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC17E96A-017B-2144-9594-2CB3CB59839B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0458AEC0-267E-8E4C-A94B-A11731DF5495}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="18060" windowHeight="13960"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="13560" windowHeight="13960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="times_RCA_PDD_DSA_ECDSA" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <r>
-      <t xml:space="preserve">RSA PSS </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Cuerpo)_x0000_"/>
-      </rPr>
-      <t>Firma</t>
-    </r>
-  </si>
   <si>
     <r>
       <t xml:space="preserve">RSA PSS </t>
@@ -62,8 +49,15 @@
     </r>
   </si>
   <si>
+    <t>Tiempos Firma</t>
+  </si>
+  <si>
+    <t>Tiempos Verificación</t>
+  </si>
+  <si>
     <r>
-      <t>DSA</t>
+      <t xml:space="preserve">ECDSA 
+</t>
     </r>
     <r>
       <rPr>
@@ -71,12 +65,26 @@
         <color theme="1"/>
         <rFont val="Calibri (Cuerpo)_x0000_"/>
       </rPr>
-      <t xml:space="preserve"> Verificación</t>
+      <t>Firma</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ECDSA </t>
+      <t>RSA PSS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Cuerpo)_x0000_"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Firma</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DSA </t>
     </r>
     <r>
       <rPr>
@@ -97,21 +105,14 @@
         <color theme="1"/>
         <rFont val="Calibri (Cuerpo)_x0000_"/>
       </rPr>
-      <t xml:space="preserve"> 
-Firma</t>
+      <t xml:space="preserve"> Verificación</t>
     </r>
-  </si>
-  <si>
-    <t>Tiempos Firma</t>
-  </si>
-  <si>
-    <t>Tiempos Verificación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -617,13 +618,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,45 +979,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="32">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" ht="32">
-      <c r="A2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1360,27 +1361,27 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <f>AVERAGE(A3:A19)</f>
         <v>7.7482352941178818E-4</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <f t="shared" ref="B20:E20" si="0">AVERAGE(B3:B19)</f>
         <v>3.3176470588237271E-3</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <f t="shared" si="0"/>
         <v>1.1465882352942034E-3</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <f t="shared" si="0"/>
         <v>6.7947058823523369E-4</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f t="shared" ref="F20" si="1">AVERAGE(F3:F19)</f>
         <v>5.1177058823527743E-3</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" ref="G20" si="2">AVERAGE(G3:G19)</f>
         <v>5.6841176470605369E-4</v>
       </c>

</xml_diff>